<commit_message>
Update: Convert XLSX to JSON
</commit_message>
<xml_diff>
--- a/XLSXtoJSONorCSV/Data/sample01.xlsx
+++ b/XLSXtoJSONorCSV/Data/sample01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmitKumarSahoo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Training\projects\csharp-presentation\DataConversionApplication\ConversionConsoleApp\XLSXtoJSONorCSV\XLSXtoJSONorCSV\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38B19922-5190-4DDA-83DD-577994ECD775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FED862F-1380-422D-9DEB-CE4F4EA50E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{10C130BF-B0BF-4932-9A15-18B549FC9091}"/>
   </bookViews>
@@ -50,27 +50,6 @@
     <t>lowerwhisker</t>
   </si>
   <si>
-    <t>Explained by: Log GDP per capita</t>
-  </si>
-  <si>
-    <t>Explained by: Social support</t>
-  </si>
-  <si>
-    <t>Explained by: Healthy life expectancy</t>
-  </si>
-  <si>
-    <t>Explained by: Freedom to make life choices</t>
-  </si>
-  <si>
-    <t>Explained by: Generosity</t>
-  </si>
-  <si>
-    <t>Explained by: Perceptions of corruption</t>
-  </si>
-  <si>
-    <t>Dystopia + residual</t>
-  </si>
-  <si>
     <t>Finland</t>
   </si>
   <si>
@@ -498,6 +477,27 @@
   </si>
   <si>
     <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Generosity</t>
+  </si>
+  <si>
+    <t>LogGDPpercapita</t>
+  </si>
+  <si>
+    <t>Socialsupport</t>
+  </si>
+  <si>
+    <t>Healthylifeexpectancy</t>
+  </si>
+  <si>
+    <t>Freedomtomakelifechoices</t>
+  </si>
+  <si>
+    <t>Perceptionsofcorruption</t>
+  </si>
+  <si>
+    <t>DystopiaResidual</t>
   </si>
 </sst>
 </file>
@@ -852,10 +852,23 @@
   <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD144"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" customWidth="1"/>
+    <col min="4" max="4" width="26.90625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" customWidth="1"/>
+    <col min="8" max="8" width="22.81640625" customWidth="1"/>
+    <col min="9" max="9" width="20.54296875" customWidth="1"/>
+    <col min="10" max="10" width="21.6328125" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -871,30 +884,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>152</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>7.7409999999999997</v>
@@ -929,7 +942,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>7.5830000000000002</v>
@@ -964,7 +977,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>7.5250000000000004</v>
@@ -999,7 +1012,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>7.3440000000000003</v>
@@ -1034,7 +1047,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>7.3410000000000002</v>
@@ -1069,7 +1082,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>7.319</v>
@@ -1104,7 +1117,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7.3019999999999996</v>
@@ -1139,7 +1152,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>7.1219999999999999</v>
@@ -1174,7 +1187,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>7.06</v>
@@ -1209,7 +1222,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>7.0570000000000004</v>
@@ -1244,7 +1257,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>7.0289999999999999</v>
@@ -1279,7 +1292,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>6.9550000000000001</v>
@@ -1314,7 +1327,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>6.9509999999999996</v>
@@ -1349,7 +1362,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>6.9050000000000002</v>
@@ -1384,7 +1397,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>6.9</v>
@@ -1419,7 +1432,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>6.8940000000000001</v>
@@ -1454,7 +1467,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6.8380000000000001</v>
@@ -1489,7 +1502,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>6.8220000000000001</v>
@@ -1524,7 +1537,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>6.8179999999999996</v>
@@ -1559,7 +1572,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>6.7489999999999997</v>
@@ -1594,7 +1607,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>6.7430000000000003</v>
@@ -1629,7 +1642,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>6.7329999999999997</v>
@@ -1664,7 +1677,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>6.7249999999999996</v>
@@ -1699,7 +1712,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>6.7190000000000003</v>
@@ -1734,7 +1747,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>6.6779999999999999</v>
@@ -1769,7 +1782,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>6.6109999999999998</v>
@@ -1804,7 +1817,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>6.609</v>
@@ -1839,7 +1852,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>6.5940000000000003</v>
@@ -1874,7 +1887,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>6.5609999999999999</v>
@@ -1909,7 +1922,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>6.5229999999999997</v>
@@ -1944,7 +1957,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>6.5030000000000001</v>
@@ -1979,7 +1992,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>6.4909999999999997</v>
@@ -2014,7 +2027,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>6.4690000000000003</v>
@@ -2049,7 +2062,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>6.4480000000000004</v>
@@ -2084,7 +2097,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>6.4420000000000002</v>
@@ -2119,7 +2132,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>6.4210000000000003</v>
@@ -2154,7 +2167,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>6.4109999999999996</v>
@@ -2189,7 +2202,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>6.36</v>
@@ -2224,7 +2237,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>6.3579999999999997</v>
@@ -2259,7 +2272,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>6.3460000000000001</v>
@@ -2294,7 +2307,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>6.3239999999999998</v>
@@ -2329,7 +2342,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>6.2869999999999999</v>
@@ -2364,7 +2377,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>6.2839999999999998</v>
@@ -2399,7 +2412,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>6.2720000000000002</v>
@@ -2434,7 +2447,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>6.2569999999999997</v>
@@ -2469,7 +2482,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>6.234</v>
@@ -2504,7 +2517,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>6.1950000000000003</v>
@@ -2539,7 +2552,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>6.1879999999999997</v>
@@ -2574,7 +2587,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>6.1879999999999997</v>
@@ -2609,7 +2622,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>6.0679999999999996</v>
@@ -2644,7 +2657,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>6.06</v>
@@ -2679,7 +2692,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>6.0579999999999998</v>
@@ -2714,7 +2727,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>6.048</v>
@@ -2749,7 +2762,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>6.0430000000000001</v>
@@ -2784,7 +2797,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>6.03</v>
@@ -2819,7 +2832,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>6.0170000000000003</v>
@@ -2854,7 +2867,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>5.9770000000000003</v>
@@ -2889,7 +2902,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>5.976</v>
@@ -2924,7 +2937,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>5.9749999999999996</v>
@@ -2959,7 +2972,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>5.9729999999999999</v>
@@ -2994,7 +3007,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>5.968</v>
@@ -3029,7 +3042,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>5.9589999999999996</v>
@@ -3043,7 +3056,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>5.9420000000000002</v>
@@ -3078,7 +3091,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>5.9340000000000002</v>
@@ -3113,7 +3126,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>5.8769999999999998</v>
@@ -3148,7 +3161,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>5.8659999999999997</v>
@@ -3183,7 +3196,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>5.8419999999999996</v>
@@ -3218,7 +3231,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>5.8410000000000002</v>
@@ -3253,7 +3266,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>5.8230000000000004</v>
@@ -3288,7 +3301,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>5.8159999999999998</v>
@@ -3323,7 +3336,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>5.8159999999999998</v>
@@ -3358,7 +3371,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>5.7850000000000001</v>
@@ -3393,7 +3406,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>5.7839999999999998</v>
@@ -3428,7 +3441,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>5.7249999999999996</v>
@@ -3463,7 +3476,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>5.7140000000000004</v>
@@ -3498,7 +3511,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>5.7069999999999999</v>
@@ -3533,7 +3546,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>5.6959999999999997</v>
@@ -3568,7 +3581,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>5.6950000000000003</v>
@@ -3603,7 +3616,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>5.6070000000000002</v>
@@ -3638,7 +3651,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>5.5679999999999996</v>
@@ -3673,7 +3686,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>5.4630000000000001</v>
@@ -3708,7 +3721,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>5.4550000000000001</v>
@@ -3743,7 +3756,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>5.4219999999999997</v>
@@ -3778,7 +3791,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>5.3689999999999998</v>
@@ -3813,7 +3826,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>5.3639999999999999</v>
@@ -3848,7 +3861,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>5.3159999999999998</v>
@@ -3883,7 +3896,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>5.3040000000000003</v>
@@ -3918,7 +3931,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>5.2809999999999997</v>
@@ -3932,7 +3945,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>5.2210000000000001</v>
@@ -3967,7 +3980,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>5.2160000000000002</v>
@@ -4002,7 +4015,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>5.1849999999999996</v>
@@ -4037,7 +4050,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>5.1660000000000004</v>
@@ -4072,7 +4085,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B94">
         <v>5.1580000000000004</v>
@@ -4107,7 +4120,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>5.1390000000000002</v>
@@ -4142,7 +4155,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B96">
         <v>5.1059999999999999</v>
@@ -4177,7 +4190,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>5.08</v>
@@ -4212,7 +4225,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>5.0229999999999997</v>
@@ -4247,7 +4260,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>4.9749999999999996</v>
@@ -4282,7 +4295,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B100">
         <v>4.9690000000000003</v>
@@ -4317,7 +4330,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B101">
         <v>4.923</v>
@@ -4352,7 +4365,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B102">
         <v>4.8929999999999998</v>
@@ -4387,7 +4400,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B103">
         <v>4.8810000000000002</v>
@@ -4422,7 +4435,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B104">
         <v>4.8789999999999996</v>
@@ -4436,7 +4449,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B105">
         <v>4.8739999999999997</v>
@@ -4471,7 +4484,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B106">
         <v>4.8730000000000002</v>
@@ -4506,7 +4519,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B107">
         <v>4.8319999999999999</v>
@@ -4541,7 +4554,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B108">
         <v>4.7949999999999999</v>
@@ -4576,7 +4589,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B109">
         <v>4.657</v>
@@ -4611,7 +4624,7 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B110">
         <v>4.556</v>
@@ -4646,7 +4659,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B111">
         <v>4.548</v>
@@ -4681,7 +4694,7 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B112">
         <v>4.5049999999999999</v>
@@ -4716,7 +4729,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B113">
         <v>4.4850000000000003</v>
@@ -4751,7 +4764,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B114">
         <v>4.4710000000000001</v>
@@ -4786,7 +4799,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B115">
         <v>4.47</v>
@@ -4821,7 +4834,7 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B116">
         <v>4.4219999999999997</v>
@@ -4856,7 +4869,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B117">
         <v>4.3769999999999998</v>
@@ -4891,7 +4904,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B118">
         <v>4.3719999999999999</v>
@@ -4926,7 +4939,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B119">
         <v>4.3540000000000001</v>
@@ -4961,7 +4974,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B120">
         <v>4.3410000000000002</v>
@@ -4996,7 +5009,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B121">
         <v>4.2889999999999997</v>
@@ -5031,7 +5044,7 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B122">
         <v>4.2690000000000001</v>
@@ -5066,7 +5079,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B123">
         <v>4.2320000000000002</v>
@@ -5101,7 +5114,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B124">
         <v>4.2279999999999998</v>
@@ -5136,7 +5149,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B125">
         <v>4.2140000000000004</v>
@@ -5171,7 +5184,7 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B126">
         <v>4.1859999999999999</v>
@@ -5206,7 +5219,7 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B127">
         <v>4.0540000000000003</v>
@@ -5241,7 +5254,7 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B128">
         <v>3.9769999999999999</v>
@@ -5276,7 +5289,7 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B129">
         <v>3.8980000000000001</v>
@@ -5311,7 +5324,7 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B130">
         <v>3.8860000000000001</v>
@@ -5346,7 +5359,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>3.8610000000000002</v>
@@ -5381,7 +5394,7 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>3.7810000000000001</v>
@@ -5416,7 +5429,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>3.5659999999999998</v>
@@ -5451,7 +5464,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B134">
         <v>3.5609999999999999</v>
@@ -5486,7 +5499,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B135">
         <v>3.5019999999999998</v>
@@ -5521,7 +5534,7 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B136">
         <v>3.5019999999999998</v>
@@ -5556,7 +5569,7 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B137">
         <v>3.4209999999999998</v>
@@ -5591,7 +5604,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B138">
         <v>3.383</v>
@@ -5626,7 +5639,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B139">
         <v>3.3410000000000002</v>
@@ -5661,7 +5674,7 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B140">
         <v>3.2949999999999999</v>
@@ -5696,7 +5709,7 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B141">
         <v>3.2450000000000001</v>
@@ -5731,7 +5744,7 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B142">
         <v>3.1859999999999999</v>
@@ -5766,7 +5779,7 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B143">
         <v>2.7069999999999999</v>
@@ -5801,7 +5814,7 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B144">
         <v>1.7210000000000001</v>

</xml_diff>